<commit_message>
Change APP template size to A4
</commit_message>
<xml_diff>
--- a/app/tmp/APP_template.xlsx
+++ b/app/tmp/APP_template.xlsx
@@ -132,7 +132,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.55"/>
@@ -143,7 +143,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="5" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>